<commit_message>
Updating new Python code and correct answers
</commit_message>
<xml_diff>
--- a/Sales_Data/monthly_totals_2019.xlsx
+++ b/Sales_Data/monthly_totals_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5c3faf0438cc858a/Desktop/Business Analysis/sales_analysis_python/Sales_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{2EF5F691-9A88-4354-A10B-C72C3FD43F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76BA4DB9-8DB0-4E91-A769-C0FE73B4802E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{2EF5F691-9A88-4354-A10B-C72C3FD43F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D252FF53-A93C-45D0-B32B-7B08CB8B2E71}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A35B19A2-6523-415C-B3BE-820E6B62C631}"/>
+    <workbookView minimized="1" xWindow="9435" yWindow="3780" windowWidth="7500" windowHeight="6000" xr2:uid="{A35B19A2-6523-415C-B3BE-820E6B62C631}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -130,6 +130,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>